<commit_message>
2016.2 updates. Maybe the last ones
</commit_message>
<xml_diff>
--- a/data/Item List E10.xlsx
+++ b/data/Item List E10.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25915"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\beaker\Profound Decisions\Odyssey\10 - River of Night's Dreaming\Dropbox\10 - The River of Night's Dreaming\Artifacts, Blessings and Curses\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="16380" windowHeight="8200" activeTab="1"/>
+    <workbookView xWindow="8370" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Tribute and Pack Items" sheetId="1" r:id="rId1"/>
@@ -12,17 +17,12 @@
     <sheet name="Ribbon numbers" sheetId="4" r:id="rId3"/>
     <sheet name="Tables" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="537">
   <si>
     <t>Ribbon #</t>
   </si>
@@ -1783,61 +1783,16 @@
     <t>quest</t>
   </si>
   <si>
-    <t xml:space="preserve">When a liquid is placed inside this item and then poured 20 drachma, an ingot of Orichalcum is produced. The character who has activated the item has the following roleplay effect: You feel acquisitive and inclined to seek out wealth and luxury. This effect lasts a few minutes and may recur at your discretion. </t>
-  </si>
-  <si>
-    <t>Smells of hot metal</t>
-  </si>
-  <si>
-    <t>crucible</t>
-  </si>
-  <si>
-    <t>Chancellery NPC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A pale face stirring a metal crucible, muttering words, drawing blood from another with a wicked-looking dagger.  </t>
-  </si>
-  <si>
-    <t>Metal vessel</t>
-  </si>
-  <si>
-    <t>metal vessel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plot item </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When a liquid is placed inside this item and then poured 20 drachma, an ingot of Electrum is produced. The character who has activated the item has the following roleplay effect: You feel inquisitive and inclined to seek out knowledge and new experiences. This effect lasts a few minutes and may recur at your discretion. </t>
-  </si>
-  <si>
-    <t>smells of hot metal</t>
-  </si>
-  <si>
-    <t>dark bottle</t>
-  </si>
-  <si>
-    <t>plot item</t>
-  </si>
-  <si>
-    <t>When a liquid is placed inside this item and then poured over coin, an ingot of Hepatizon is produced. The character who has activated the item has the following roleplay effect: You feel cultured and inclined to seek out beauty and creative endeavour. This effect lasts a few minutes and may recur at your discretion. Descriptor text: Smells of hot metal</t>
-  </si>
-  <si>
-    <t>small bottle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When a liquid is placed inside this item and then poured over coin, a small quantity of Thocture is produced. The character who has activated the item has the following roleplay effect: You feel exhilarated and inclined to seek out excitement and activity. </t>
-  </si>
-  <si>
-    <t>ancient crucible</t>
-  </si>
-  <si>
-    <t>small ancient crucible</t>
-  </si>
-  <si>
-    <t>bottle</t>
-  </si>
-  <si>
-    <t>A pale face stirring a metal crucible, muttering words, drawing blood from another with a wicked-looking dagger</t>
+    <t>Potion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A clear liquid, smelling faintly of juniper. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">potion  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This potion may only be taken by a Persian Warleader. It provides a calming and soothing influence on the drinker and allows them to call RESIST to any imposed roleplaying effect. It is suggested that it is phys-repped with a liberal shot of gin and tonic. </t>
   </si>
   <si>
     <t>This item can only be used by a GREEK PRIEST OR ATTENDANT. The priest gains the use of the skill USE ONE-HANDED WEAPON With respect to this sword only. The weilder may enter the arena and fight with their warband as if they were a champion. The priest may use the sword to strike for PARALYZE once OR REPEL three times during one arena battle - once used, this power is then expended and cannot be used again at THE RIVER OF NIGHTS DREAMING. The sword may not be taken on a quest. Using this sword in the arena will draw the attention of PHOBOS and DEIMOS onto the user. If the sword is not used to0 strike a blow against an enemy in every arena combat it enters, or if it does not enter an arena combat for the entire Annual, the wielder becomes subject ot the CURSE OF DEIMOS. It may be used to execute a Gorgon</t>
@@ -1847,7 +1802,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1942,12 +1897,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1995,7 +1944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2056,7 +2005,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2117,7 +2065,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2152,7 +2100,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2329,7 +2277,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2337,21 +2285,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="27.5703125"/>
+    <col min="3" max="3" width="8.7109375"/>
+    <col min="4" max="4" width="54.85546875"/>
+    <col min="5" max="5" width="15.140625"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="33.28515625"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2386,7 +2341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="409">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="179.25" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>42</v>
@@ -2422,7 +2377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="409">
+    <row r="3" spans="1:11" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>40</v>
@@ -2456,7 +2411,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>153</v>
       </c>
@@ -2488,7 +2443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>105</v>
@@ -2520,7 +2475,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="409">
+    <row r="6" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>14</v>
@@ -2556,7 +2511,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="409">
+    <row r="7" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>43</v>
@@ -2592,7 +2547,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>44</v>
@@ -2623,7 +2578,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="409">
+    <row r="9" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27</v>
       </c>
@@ -2658,7 +2613,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="409">
+    <row r="10" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>25</v>
@@ -2694,7 +2649,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="409">
+    <row r="11" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>12</v>
@@ -2730,7 +2685,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="409">
+    <row r="12" spans="1:11" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>10</v>
@@ -2766,7 +2721,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="409">
+    <row r="13" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>9</v>
@@ -2802,7 +2757,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="409">
+    <row r="14" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>23</v>
       </c>
@@ -2837,7 +2792,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="409">
+    <row r="15" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>97</v>
@@ -2873,7 +2828,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>47</v>
@@ -2909,7 +2864,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="409">
+    <row r="17" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>4</v>
@@ -2945,7 +2900,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="409">
+    <row r="18" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>15</v>
@@ -2978,7 +2933,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="409">
+    <row r="19" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>7</v>
@@ -3014,7 +2969,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="409">
+    <row r="20" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>51</v>
@@ -3047,7 +3002,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="409">
+    <row r="21" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>6</v>
@@ -3083,7 +3038,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="409">
+    <row r="22" spans="1:11" ht="255.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -3118,7 +3073,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>1</v>
@@ -3149,7 +3104,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="409">
+    <row r="24" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>2</v>
@@ -3185,7 +3140,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3220,7 +3175,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="409">
+    <row r="26" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8</v>
       </c>
@@ -3255,7 +3210,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="409">
+    <row r="27" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>5</v>
@@ -3291,7 +3246,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="364">
+    <row r="28" spans="1:11" ht="217.5" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>22</v>
@@ -3327,7 +3282,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="409">
+    <row r="29" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>21</v>
@@ -3363,7 +3318,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="409">
+    <row r="30" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>30</v>
@@ -3399,7 +3354,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>28</v>
@@ -3435,7 +3390,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>29</v>
@@ -3471,7 +3426,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>31</v>
@@ -3507,7 +3462,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>37</v>
@@ -3543,7 +3498,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>38</v>
@@ -3579,7 +3534,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="409">
+    <row r="36" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>36</v>
@@ -3615,7 +3570,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>39</v>
       </c>
@@ -3650,7 +3605,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -3685,7 +3640,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>34</v>
       </c>
@@ -3720,7 +3675,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="409">
+    <row r="40" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>32</v>
       </c>
@@ -3755,7 +3710,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>33</v>
@@ -3791,7 +3746,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="409">
+    <row r="42" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>53</v>
@@ -3827,7 +3782,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="409">
+    <row r="43" spans="1:11" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>26</v>
@@ -3860,7 +3815,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>142</v>
@@ -3894,7 +3849,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="409">
+    <row r="45" spans="1:11" ht="281.25" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>41</v>
@@ -3930,7 +3885,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="409">
+    <row r="46" spans="1:11" ht="255.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>11</v>
@@ -3966,7 +3921,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="409">
+    <row r="47" spans="1:11" ht="141" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>VLOOKUP(B:B,'Ribbon numbers'!B:G,6,FALSE)</f>
         <v>90</v>
@@ -4002,7 +3957,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="409">
+    <row r="48" spans="1:11" ht="179.25" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>160</v>
       </c>
@@ -4028,7 +3983,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="409">
+    <row r="49" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>171</v>
       </c>
@@ -4057,28 +4012,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="36.7109375"/>
+    <col min="3" max="3" width="8.7109375"/>
+    <col min="4" max="4" width="47.7109375"/>
+    <col min="5" max="5" width="38.7109375"/>
+    <col min="6" max="8" width="8.7109375"/>
+    <col min="9" max="9" width="28.5703125"/>
+    <col min="10" max="1025" width="8.7109375"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4113,7 +4073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="409">
+    <row r="2" spans="1:11" ht="141" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>154</v>
       </c>
@@ -4140,7 +4100,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="409">
+    <row r="3" spans="1:11" ht="192" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>110</v>
       </c>
@@ -4151,7 +4111,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>253</v>
@@ -4172,7 +4132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="409">
+    <row r="4" spans="1:11" ht="396" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>109</v>
       </c>
@@ -4199,7 +4159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>56</v>
       </c>
@@ -4228,7 +4188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>111</v>
       </c>
@@ -4257,7 +4217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="409">
+    <row r="7" spans="1:11" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>54</v>
       </c>
@@ -4289,7 +4249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28">
+    <row r="8" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>127</v>
       </c>
@@ -4316,7 +4276,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="409">
+    <row r="9" spans="1:11" ht="141" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>128</v>
       </c>
@@ -4343,7 +4303,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28">
+    <row r="10" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>129</v>
       </c>
@@ -4370,7 +4330,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28">
+    <row r="11" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>130</v>
       </c>
@@ -4397,7 +4357,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>131</v>
       </c>
@@ -4424,7 +4384,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="42">
+    <row r="13" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>132</v>
       </c>
@@ -4451,7 +4411,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28">
+    <row r="14" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>66</v>
       </c>
@@ -4483,7 +4443,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="28">
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>135</v>
       </c>
@@ -4512,7 +4472,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28">
+    <row r="16" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>155</v>
       </c>
@@ -4541,7 +4501,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>156</v>
       </c>
@@ -4570,7 +4530,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>157</v>
       </c>
@@ -4599,7 +4559,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="28">
+    <row r="19" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>158</v>
       </c>
@@ -4628,7 +4588,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>58</v>
       </c>
@@ -4654,7 +4614,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>59</v>
       </c>
@@ -4686,7 +4646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>104</v>
       </c>
@@ -4714,7 +4674,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>145</v>
       </c>
@@ -4741,7 +4701,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>149</v>
       </c>
@@ -4766,7 +4726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>150</v>
       </c>
@@ -4791,7 +4751,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28">
+    <row r="26" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>159</v>
       </c>
@@ -4814,7 +4774,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="250">
+    <row r="27" spans="1:10" ht="139.5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>161</v>
       </c>
@@ -4840,7 +4800,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>162</v>
       </c>
@@ -4869,7 +4829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>163</v>
       </c>
@@ -4898,7 +4858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>164</v>
       </c>
@@ -4927,7 +4887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>165</v>
       </c>
@@ -4956,7 +4916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>166</v>
       </c>
@@ -4985,7 +4945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>167</v>
       </c>
@@ -5014,7 +4974,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>168</v>
       </c>
@@ -5043,7 +5003,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>169</v>
       </c>
@@ -5072,7 +5032,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>170</v>
       </c>
@@ -5101,7 +5061,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>172</v>
       </c>
@@ -5127,7 +5087,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>173</v>
       </c>
@@ -5153,181 +5113,54 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>174</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="34" t="s">
-        <v>532</v>
+      <c r="D39" s="3" t="s">
+        <v>535</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>538</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>535</v>
-      </c>
       <c r="H39" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="34" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40">
-        <v>175</v>
-      </c>
-      <c r="B40" s="31" t="s">
-        <v>548</v>
-      </c>
-      <c r="C40" t="s">
-        <v>539</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>540</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>534</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="H40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="34" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41">
-        <v>176</v>
-      </c>
-      <c r="B41" s="31" t="s">
-        <v>542</v>
-      </c>
-      <c r="C41" t="s">
-        <v>543</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>544</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>533</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="H41" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="34" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42">
-        <v>177</v>
-      </c>
-      <c r="B42" s="31" t="s">
-        <v>545</v>
-      </c>
-      <c r="C42" t="s">
-        <v>543</v>
-      </c>
-      <c r="D42" s="34" t="s">
-        <v>546</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="H42" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="34" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43">
-        <v>178</v>
-      </c>
-      <c r="B43" s="31" t="s">
-        <v>547</v>
-      </c>
-      <c r="C43" t="s">
-        <v>543</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>550</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>534</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="H43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="34" t="s">
-        <v>536</v>
+        <v>34</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
     <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="L175" sqref="L175"/>
+      <selection activeCell="H182" sqref="H182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="7" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>338</v>
       </c>
@@ -5350,7 +5183,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -5373,7 +5206,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-1</v>
       </c>
@@ -5396,7 +5229,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5419,7 +5252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -5442,7 +5275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -5465,7 +5298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -5488,7 +5321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -5511,7 +5344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -5534,7 +5367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -5557,7 +5390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -5580,7 +5413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -5603,7 +5436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -5626,7 +5459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -5649,7 +5482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -5672,7 +5505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -5695,7 +5528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -5718,7 +5551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -5741,7 +5574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -5764,7 +5597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -5787,7 +5620,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5810,7 +5643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5833,7 +5666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5856,7 +5689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -5879,7 +5712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -5902,7 +5735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -5925,7 +5758,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -5948,7 +5781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -5971,7 +5804,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -5994,7 +5827,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -6017,7 +5850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -6040,7 +5873,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -6063,7 +5896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -6086,7 +5919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -6109,7 +5942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -6132,7 +5965,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -6155,7 +5988,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -6178,7 +6011,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -6201,7 +6034,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -6224,7 +6057,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -6247,7 +6080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -6270,7 +6103,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -6293,7 +6126,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -6316,7 +6149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -6339,7 +6172,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -6362,7 +6195,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -6385,7 +6218,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -6408,7 +6241,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -6431,7 +6264,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -6454,7 +6287,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -6477,7 +6310,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
@@ -6500,7 +6333,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -6523,7 +6356,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -6546,7 +6379,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -6569,7 +6402,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -6592,7 +6425,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -6615,7 +6448,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -6638,7 +6471,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -6661,7 +6494,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -6684,7 +6517,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -6707,7 +6540,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -6730,7 +6563,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -6753,7 +6586,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
@@ -6776,7 +6609,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
@@ -6799,7 +6632,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62</v>
       </c>
@@ -6822,7 +6655,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>63</v>
       </c>
@@ -6845,7 +6678,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>64</v>
       </c>
@@ -6868,7 +6701,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>65</v>
       </c>
@@ -6891,7 +6724,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>66</v>
       </c>
@@ -6914,7 +6747,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
@@ -6937,7 +6770,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
@@ -6960,7 +6793,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
@@ -6983,7 +6816,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
@@ -7006,7 +6839,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
@@ -7029,7 +6862,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
@@ -7052,7 +6885,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
@@ -7075,7 +6908,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
@@ -7098,7 +6931,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
@@ -7121,7 +6954,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
@@ -7144,7 +6977,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>77</v>
       </c>
@@ -7167,7 +7000,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
@@ -7190,7 +7023,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>79</v>
       </c>
@@ -7213,7 +7046,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>80</v>
       </c>
@@ -7236,7 +7069,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>81</v>
       </c>
@@ -7259,7 +7092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>82</v>
       </c>
@@ -7282,7 +7115,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>83</v>
       </c>
@@ -7305,7 +7138,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>84</v>
       </c>
@@ -7328,7 +7161,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>85</v>
       </c>
@@ -7351,7 +7184,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>86</v>
       </c>
@@ -7374,7 +7207,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>87</v>
       </c>
@@ -7397,7 +7230,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>88</v>
       </c>
@@ -7420,7 +7253,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>89</v>
       </c>
@@ -7443,7 +7276,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>90</v>
       </c>
@@ -7466,7 +7299,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>91</v>
       </c>
@@ -7489,7 +7322,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>92</v>
       </c>
@@ -7512,7 +7345,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>93</v>
       </c>
@@ -7535,7 +7368,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>94</v>
       </c>
@@ -7558,7 +7391,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>95</v>
       </c>
@@ -7581,7 +7414,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>96</v>
       </c>
@@ -7604,7 +7437,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>97</v>
       </c>
@@ -7627,7 +7460,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>98</v>
       </c>
@@ -7650,7 +7483,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>99</v>
       </c>
@@ -7673,7 +7506,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>100</v>
       </c>
@@ -7696,7 +7529,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>101</v>
       </c>
@@ -7719,7 +7552,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>102</v>
       </c>
@@ -7742,7 +7575,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>103</v>
       </c>
@@ -7765,7 +7598,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>104</v>
       </c>
@@ -7788,7 +7621,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>105</v>
       </c>
@@ -7811,7 +7644,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>106</v>
       </c>
@@ -7834,7 +7667,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>107</v>
       </c>
@@ -7857,7 +7690,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>108</v>
       </c>
@@ -7880,7 +7713,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>109</v>
       </c>
@@ -7903,7 +7736,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>110</v>
       </c>
@@ -7926,7 +7759,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>111</v>
       </c>
@@ -7949,7 +7782,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>112</v>
       </c>
@@ -7972,7 +7805,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>113</v>
       </c>
@@ -7995,7 +7828,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>114</v>
       </c>
@@ -8018,7 +7851,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>115</v>
       </c>
@@ -8041,7 +7874,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>116</v>
       </c>
@@ -8064,7 +7897,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>117</v>
       </c>
@@ -8087,7 +7920,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>118</v>
       </c>
@@ -8110,7 +7943,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>119</v>
       </c>
@@ -8133,7 +7966,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>120</v>
       </c>
@@ -8156,7 +7989,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>121</v>
       </c>
@@ -8179,7 +8012,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>122</v>
       </c>
@@ -8202,7 +8035,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>123</v>
       </c>
@@ -8225,7 +8058,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>124</v>
       </c>
@@ -8248,7 +8081,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>125</v>
       </c>
@@ -8271,7 +8104,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>126</v>
       </c>
@@ -8294,7 +8127,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>127</v>
       </c>
@@ -8317,7 +8150,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>128</v>
       </c>
@@ -8340,7 +8173,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>129</v>
       </c>
@@ -8363,7 +8196,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>130</v>
       </c>
@@ -8386,7 +8219,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>131</v>
       </c>
@@ -8409,7 +8242,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>132</v>
       </c>
@@ -8432,7 +8265,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>133</v>
       </c>
@@ -8455,7 +8288,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>134</v>
       </c>
@@ -8478,7 +8311,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>135</v>
       </c>
@@ -8501,7 +8334,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>136</v>
       </c>
@@ -8524,7 +8357,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>137</v>
       </c>
@@ -8547,7 +8380,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>138</v>
       </c>
@@ -8570,7 +8403,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>139</v>
       </c>
@@ -8593,7 +8426,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>140</v>
       </c>
@@ -8616,7 +8449,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>141</v>
       </c>
@@ -8639,7 +8472,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>142</v>
       </c>
@@ -8662,7 +8495,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>143</v>
       </c>
@@ -8685,7 +8518,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>144</v>
       </c>
@@ -8708,7 +8541,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>145</v>
       </c>
@@ -8731,7 +8564,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>146</v>
       </c>
@@ -8754,7 +8587,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>147</v>
       </c>
@@ -8777,7 +8610,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>148</v>
       </c>
@@ -8800,7 +8633,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>149</v>
       </c>
@@ -8823,7 +8656,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>150</v>
       </c>
@@ -8846,7 +8679,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>151</v>
       </c>
@@ -8869,7 +8702,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>152</v>
       </c>
@@ -8892,7 +8725,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="29">
         <v>153</v>
       </c>
@@ -8915,7 +8748,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="29">
         <v>154</v>
       </c>
@@ -8938,7 +8771,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="29">
         <v>155</v>
       </c>
@@ -8961,7 +8794,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="29">
         <v>156</v>
       </c>
@@ -8984,7 +8817,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="29">
         <v>157</v>
       </c>
@@ -9007,7 +8840,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="29">
         <v>158</v>
       </c>
@@ -9030,7 +8863,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="29">
         <v>159</v>
       </c>
@@ -9053,7 +8886,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="29">
         <v>160</v>
       </c>
@@ -9076,7 +8909,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="29">
         <v>161</v>
       </c>
@@ -9099,7 +8932,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="29">
         <v>162</v>
       </c>
@@ -9122,7 +8955,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="29">
         <v>163</v>
       </c>
@@ -9145,7 +8978,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="29">
         <v>164</v>
       </c>
@@ -9168,7 +9001,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="29">
         <v>165</v>
       </c>
@@ -9191,7 +9024,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="29">
         <v>166</v>
       </c>
@@ -9214,7 +9047,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="29">
         <v>167</v>
       </c>
@@ -9237,7 +9070,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="29">
         <v>168</v>
       </c>
@@ -9260,7 +9093,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="29">
         <v>169</v>
       </c>
@@ -9283,7 +9116,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="29">
         <v>170</v>
       </c>
@@ -9306,7 +9139,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="29">
         <v>171</v>
       </c>
@@ -9329,7 +9162,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="29">
         <v>172</v>
       </c>
@@ -9352,7 +9185,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="29">
         <v>173</v>
       </c>
@@ -9373,6 +9206,29 @@
       </c>
       <c r="G176" s="29">
         <v>173</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="29">
+        <v>174</v>
+      </c>
+      <c r="B177" s="30" t="s">
+        <v>534</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+      <c r="F177">
+        <v>1</v>
+      </c>
+      <c r="G177" s="29">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -9380,64 +9236,62 @@
     <sortCondition ref="M9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="8.7109375"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>336</v>
       </c>
@@ -9445,10 +9299,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>